<commit_message>
Reformat PAF plot code, change exposures for aOR table, and create separate PAF and aOR plots
</commit_message>
<xml_diff>
--- a/data/risk-factors.xlsx
+++ b/data/risk-factors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Documents\Repos\EPM307AA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B3920C-31F4-419B-B913-B7AF1A6FFA69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA331F08-CE4F-4E0F-9A5F-79136576CFFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E8CDFC4F-9EE7-4087-83BA-FDD8F9306456}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{E8CDFC4F-9EE7-4087-83BA-FDD8F9306456}"/>
   </bookViews>
   <sheets>
     <sheet name="PAF" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="42">
   <si>
     <t>Study</t>
   </si>
@@ -155,16 +155,16 @@
     <t>aOR</t>
   </si>
   <si>
-    <t>Caveat</t>
-  </si>
-  <si>
-    <t>[On discharge]</t>
-  </si>
-  <si>
-    <t>[During final 2w]</t>
-  </si>
-  <si>
-    <t>[Relative to back]</t>
+    <t>Smoking during final 2w of pregnancy</t>
+  </si>
+  <si>
+    <t>Not exclusively breast feeding on discharge</t>
+  </si>
+  <si>
+    <t>Prone sleeping position relative to back</t>
+  </si>
+  <si>
+    <t>Prone sleeping position relative to other</t>
   </si>
 </sst>
 </file>
@@ -620,12 +620,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DB48E00E-3E5D-49A4-B5A6-432E15D3E4EB}" name="Table27" displayName="Table27" ref="A1:F10" totalsRowShown="0">
-  <autoFilter ref="A1:F10" xr:uid="{F0EE9845-9698-41CF-9334-353DC3773025}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DB48E00E-3E5D-49A4-B5A6-432E15D3E4EB}" name="Table27" displayName="Table27" ref="A1:E10" totalsRowShown="0">
+  <autoFilter ref="A1:E10" xr:uid="{F0EE9845-9698-41CF-9334-353DC3773025}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{5E746EE4-87A5-4A94-96D1-E437022F5341}" name="Exposure"/>
     <tableColumn id="2" xr3:uid="{D5F38101-CEF0-41F0-9C36-A62C49FD1004}" name="Study"/>
-    <tableColumn id="7" xr3:uid="{8F2AF221-84C1-4465-B8C4-67F5ED8B04CF}" name="Caveat"/>
     <tableColumn id="4" xr3:uid="{8C4D0882-B01B-4AEF-83AA-3509E3242D7F}" name="aOR"/>
     <tableColumn id="5" xr3:uid="{83D3DBAA-21DF-47B8-94A1-7F989F799287}" name="Lower CI" dataDxfId="40"/>
     <tableColumn id="6" xr3:uid="{C220C0E5-94B8-429D-8EC1-B84CA5918D9A}" name="Upper CI"/>
@@ -1013,7 +1012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AA4A0F-DD93-4441-A732-C9855F864F33}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -1278,22 +1277,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C495ACA-EA3A-4CB3-887B-534AF071F5B5}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1301,177 +1299,165 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2" s="1">
         <v>1.79</v>
       </c>
+      <c r="D2" s="2">
+        <v>1.3</v>
+      </c>
       <c r="E2" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="F2" s="2">
         <v>2.48</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3">
+      <c r="C3" s="3">
         <v>2.02</v>
       </c>
+      <c r="D3" s="2">
+        <v>1.35</v>
+      </c>
       <c r="E3" s="2">
-        <v>1.35</v>
-      </c>
-      <c r="F3" s="2">
         <v>3.04</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3">
+      <c r="C4" s="3">
         <v>4.84</v>
       </c>
+      <c r="D4" s="2">
+        <v>3.59</v>
+      </c>
       <c r="E4" s="2">
-        <v>3.59</v>
-      </c>
-      <c r="F4" s="2">
         <v>6.52</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="C5" s="3">
         <v>1.89</v>
       </c>
-      <c r="E5" s="2">
+      <c r="D5" s="2">
         <v>1.35</v>
       </c>
-      <c r="F5" s="1">
+      <c r="E5" s="1">
         <v>2.64</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
+      <c r="C6" s="11">
+        <v>6.01</v>
+      </c>
       <c r="D6" s="11">
-        <v>6.01</v>
+        <v>2.97</v>
       </c>
       <c r="E6" s="11">
-        <v>2.97</v>
-      </c>
-      <c r="F6" s="11">
         <v>12.15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
+      <c r="C7">
+        <v>4.96</v>
+      </c>
       <c r="D7">
-        <v>4.96</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="E7">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="F7">
         <v>9.64</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
-        <v>41</v>
+      <c r="C8">
+        <v>3.85</v>
       </c>
       <c r="D8">
-        <v>3.85</v>
+        <v>1.07</v>
       </c>
       <c r="E8">
-        <v>1.07</v>
-      </c>
-      <c r="F8">
         <v>13.89</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
+      <c r="C9" s="11">
+        <v>1.53</v>
+      </c>
       <c r="D9" s="11">
-        <v>1.53</v>
+        <v>0.45</v>
       </c>
       <c r="E9" s="11">
-        <v>0.45</v>
-      </c>
-      <c r="F9" s="11">
         <v>5.24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="D10">
+      <c r="C10">
         <v>2.77</v>
       </c>
+      <c r="D10" s="9">
+        <v>1.45</v>
+      </c>
       <c r="E10" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="F10" s="9">
         <v>5.3</v>
       </c>
     </row>

</xml_diff>